<commit_message>
test #8: Modelos finales de tests tras el filtro de celdas vacías de los excel importados
</commit_message>
<xml_diff>
--- a/decide/census/testImport.xlsx
+++ b/decide/census/testImport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t xml:space="preserve">voting_id</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t xml:space="preserve">Rubén</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nico</t>
   </si>
 </sst>
 </file>
@@ -153,13 +150,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -229,20 +226,6 @@
       </c>
       <c r="D5" s="1" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>